<commit_message>
solved Objecten IV en HU hebben een andere kolomindeling en zijn niet samen te voegen met de andere tabellen Feedback op tabellen 5.1 #641
</commit_message>
<xml_diff>
--- a/tabellen/concept/5.1/objectentabellen/objecten-concept-5.1-HU.xlsx
+++ b/tabellen/concept/5.1/objectentabellen/objecten-concept-5.1-HU.xlsx
@@ -1,145 +1,223 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100289\OneDrive\GitHub\NLCS\tabellen\concept\5.1\objectentabellen-verkort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingcrow-my.sharepoint.com/personal/elisabeth_devries_crow_nl/Documents/Documents/GitHub/NLCS/tabellen/concept/5.1/objectentabellen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C5B45413-9318-4F41-9E20-8A5ABA391E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{6AD5A27D-CDE5-403E-AC1C-889FB170BB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8947AA7-0D61-444C-AD7B-CD140CD11241}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0CC49CE9-02C4-49D3-9A1A-315D0F07ABEE}"/>
+    <workbookView xWindow="-51720" yWindow="3270" windowWidth="51840" windowHeight="21120" xr2:uid="{99805734-BCEB-4675-BBC8-487707AD2C7C}"/>
   </bookViews>
   <sheets>
-    <sheet name="objecten-concept-5.1-HU-hulpcon" sheetId="1" r:id="rId1"/>
+    <sheet name="objecten-concept-5.1-HU" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
+  <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>underscore</t>
+  </si>
+  <si>
+    <t>discipline</t>
+  </si>
+  <si>
+    <t>underscore2</t>
+  </si>
   <si>
     <t>hoofdgroep</t>
   </si>
   <si>
+    <t>underscore3</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>underscore4</t>
+  </si>
+  <si>
+    <t>subobject01</t>
+  </si>
+  <si>
+    <t>underscore5</t>
+  </si>
+  <si>
+    <t>subobject02</t>
+  </si>
+  <si>
+    <t>underscore6</t>
+  </si>
+  <si>
+    <t>subobject03</t>
+  </si>
+  <si>
+    <t>underscore7</t>
+  </si>
+  <si>
+    <t>subobject04</t>
+  </si>
+  <si>
+    <t>underscore8</t>
+  </si>
+  <si>
+    <t>subobject05</t>
+  </si>
+  <si>
+    <t>streepje</t>
+  </si>
+  <si>
+    <t>bewerking</t>
+  </si>
+  <si>
+    <t>streepje2</t>
+  </si>
+  <si>
+    <t>schaal</t>
+  </si>
+  <si>
+    <t>aobject</t>
+  </si>
+  <si>
+    <t>sobject</t>
+  </si>
+  <si>
+    <t>laagnaam</t>
+  </si>
+  <si>
+    <t>lw_b</t>
+  </si>
+  <si>
+    <t>kl_b</t>
+  </si>
+  <si>
+    <t>kl_b_a</t>
+  </si>
+  <si>
+    <t>kl_b_gd</t>
+  </si>
+  <si>
+    <t>kl_b_gn</t>
+  </si>
+  <si>
+    <t>kl_b_v</t>
+  </si>
+  <si>
+    <t>lt_b</t>
+  </si>
+  <si>
+    <t>lw_n</t>
+  </si>
+  <si>
+    <t>kl_n</t>
+  </si>
+  <si>
+    <t>kl_n_a</t>
+  </si>
+  <si>
+    <t>kl_n_gd</t>
+  </si>
+  <si>
+    <t>kl_n_gn</t>
+  </si>
+  <si>
+    <t>kl_n_v</t>
+  </si>
+  <si>
+    <t>lt_n</t>
+  </si>
+  <si>
+    <t>lw_v</t>
+  </si>
+  <si>
+    <t>kl_v</t>
+  </si>
+  <si>
+    <t>kl_v_a</t>
+  </si>
+  <si>
+    <t>kl_v_gd</t>
+  </si>
+  <si>
+    <t>kl_v_gn</t>
+  </si>
+  <si>
+    <t>kl_v_v</t>
+  </si>
+  <si>
+    <t>lt_v</t>
+  </si>
+  <si>
+    <t>lw_t</t>
+  </si>
+  <si>
+    <t>kl_t</t>
+  </si>
+  <si>
+    <t>kl_t_a</t>
+  </si>
+  <si>
+    <t>kl_t_gd</t>
+  </si>
+  <si>
+    <t>kl_t_gn</t>
+  </si>
+  <si>
+    <t>kl_t_v</t>
+  </si>
+  <si>
+    <t>lt_t</t>
+  </si>
+  <si>
+    <t>vrkl_kort</t>
+  </si>
+  <si>
+    <t>vrkl_lang</t>
+  </si>
+  <si>
     <t>id_nummer</t>
   </si>
   <si>
-    <t>omschrijving</t>
-  </si>
-  <si>
     <t>kind_van</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>discipline</t>
-  </si>
-  <si>
-    <t>lw_b</t>
-  </si>
-  <si>
-    <t>kl_b</t>
-  </si>
-  <si>
-    <t>kl_b_a</t>
-  </si>
-  <si>
-    <t>kl_b_gd</t>
-  </si>
-  <si>
-    <t>kl_b_gn</t>
-  </si>
-  <si>
-    <t>kl_b_v</t>
-  </si>
-  <si>
-    <t>lt_b</t>
-  </si>
-  <si>
-    <t>lw_n</t>
-  </si>
-  <si>
-    <t>kl_n</t>
-  </si>
-  <si>
-    <t>kl_n_a</t>
-  </si>
-  <si>
-    <t>kl_n_gd</t>
-  </si>
-  <si>
-    <t>kl_n_gn</t>
-  </si>
-  <si>
-    <t>kl_n_v</t>
-  </si>
-  <si>
-    <t>lt_n</t>
-  </si>
-  <si>
-    <t>lw_t</t>
-  </si>
-  <si>
-    <t>kl_t</t>
-  </si>
-  <si>
-    <t>kl_t_a</t>
-  </si>
-  <si>
-    <t>kl_t_gd</t>
-  </si>
-  <si>
-    <t>kl_t_gn</t>
-  </si>
-  <si>
-    <t>kl_t_v</t>
-  </si>
-  <si>
-    <t>lt_t</t>
-  </si>
-  <si>
-    <t>lw_v</t>
-  </si>
-  <si>
-    <t>kl_v</t>
-  </si>
-  <si>
-    <t>kl_v_a</t>
-  </si>
-  <si>
-    <t>kl_v_gd</t>
-  </si>
-  <si>
-    <t>kl_v_gn</t>
-  </si>
-  <si>
-    <t>kl_v_v</t>
-  </si>
-  <si>
-    <t>lt_v</t>
-  </si>
-  <si>
-    <t>element</t>
-  </si>
-  <si>
-    <t>vrkl_kort</t>
+    <t>objectURI</t>
+  </si>
+  <si>
+    <t>kind_vanURI</t>
+  </si>
+  <si>
+    <t>HULPCONSTRUCTIES</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
   <si>
     <t>HU</t>
   </si>
   <si>
-    <t>HULPCONSTRUCTIES</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>**</t>
+    <t>ACO</t>
+  </si>
+  <si>
+    <t>*_**_HU_HULPCONSTRUCTIES</t>
   </si>
   <si>
     <t>0.18</t>
@@ -152,6 +230,12 @@
   </si>
   <si>
     <t>V-CONTINUOUS-SO</t>
+  </si>
+  <si>
+    <t>http://digitalbuildingdata.tech/nlcs/def/d8c25d21-898c-4612-8c77-8ca8d07a8992</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -635,8 +719,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1011,19 +1096,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546C9388-555E-42A7-8512-B09557FD9452}">
-  <dimension ref="A1:AJ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D8B75A-F06F-48D3-8632-E92B479C5687}">
+  <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1132,109 +1219,221 @@
       <c r="AJ1" t="s">
         <v>35</v>
       </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2">
+        <v>7</v>
+      </c>
+      <c r="AB2">
+        <v>252</v>
+      </c>
+      <c r="AC2">
+        <v>130</v>
+      </c>
+      <c r="AD2">
+        <v>10</v>
+      </c>
+      <c r="AE2">
+        <v>253</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH2">
+        <v>7</v>
+      </c>
+      <c r="AI2">
+        <v>252</v>
+      </c>
+      <c r="AJ2">
+        <v>130</v>
+      </c>
+      <c r="AK2">
+        <v>10</v>
+      </c>
+      <c r="AL2">
+        <v>253</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO2">
+        <v>7</v>
+      </c>
+      <c r="AP2">
+        <v>252</v>
+      </c>
+      <c r="AQ2">
+        <v>130</v>
+      </c>
+      <c r="AR2">
+        <v>10</v>
+      </c>
+      <c r="AS2">
+        <v>253</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV2">
+        <v>7</v>
+      </c>
+      <c r="AW2">
+        <v>252</v>
+      </c>
+      <c r="AX2">
+        <v>130</v>
+      </c>
+      <c r="AY2">
+        <v>10</v>
+      </c>
+      <c r="AZ2">
+        <v>253</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD2">
         <v>2810</v>
       </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>252</v>
-      </c>
-      <c r="J2">
-        <v>130</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>253</v>
-      </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2">
-        <v>7</v>
-      </c>
-      <c r="P2">
-        <v>252</v>
-      </c>
-      <c r="Q2">
-        <v>130</v>
-      </c>
-      <c r="R2">
-        <v>10</v>
-      </c>
-      <c r="S2">
-        <v>253</v>
-      </c>
-      <c r="T2" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2">
-        <v>7</v>
-      </c>
-      <c r="W2">
-        <v>252</v>
-      </c>
-      <c r="X2">
-        <v>130</v>
-      </c>
-      <c r="Y2">
-        <v>10</v>
-      </c>
-      <c r="Z2">
-        <v>253</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC2">
-        <v>7</v>
-      </c>
-      <c r="AD2">
-        <v>252</v>
-      </c>
-      <c r="AE2">
-        <v>130</v>
-      </c>
-      <c r="AF2">
-        <v>10</v>
-      </c>
-      <c r="AG2">
-        <v>253</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>43</v>
+      <c r="BF2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>